<commit_message>
Oppdatering ihht. nye navn, samt nye variabelvalg (figurer)
</commit_message>
<xml_diff>
--- a/doc/Mapping til norske navnOK.xlsx
+++ b/doc/Mapping til norske navnOK.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="194">
   <si>
     <t>LapNumHjelpeinnstikk</t>
   </si>
@@ -532,9 +532,6 @@
     <t>HovedDato</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>OppflgRegStatus</t>
   </si>
   <si>
@@ -593,6 +590,12 @@
   </si>
   <si>
     <t>sjekk om det har blitt noe tull</t>
+  </si>
+  <si>
+    <t>Opf0KomplUtstyr</t>
+  </si>
+  <si>
+    <t>Opf0Status</t>
   </si>
 </sst>
 </file>
@@ -969,9 +972,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B71" sqref="B71:C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,7 +1016,7 @@
         <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1035,7 +1038,7 @@
         <v>58</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,7 +1049,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1123,7 +1126,7 @@
         <v>50</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1134,7 +1137,7 @@
         <v>53</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1145,7 +1148,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1156,7 +1159,7 @@
         <v>49</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1167,7 +1170,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1178,7 +1181,7 @@
         <v>52</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1189,7 +1192,7 @@
         <v>51</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -1223,7 +1226,7 @@
         <v>32</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1245,7 +1248,7 @@
         <v>45</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1397,7 +1400,7 @@
       </c>
       <c r="C40" s="4"/>
       <c r="D40" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1617,7 +1620,7 @@
         <v>6</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1686,7 +1689,7 @@
         <v>159</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1737,19 +1740,19 @@
       <c r="A71" t="s">
         <v>151</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C71" t="s">
-        <v>172</v>
+      <c r="C71" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="D71" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>166</v>
@@ -1760,18 +1763,18 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>167</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>168</v>
@@ -1782,35 +1785,35 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>169</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>170</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Alt innhold på plass i samledokument. Mangler layout...
</commit_message>
<xml_diff>
--- a/doc/Mapping til norske navnOK.xlsx
+++ b/doc/Mapping til norske navnOK.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="201">
   <si>
     <t>LapNumHjelpeinnstikk</t>
   </si>
@@ -334,9 +334,6 @@
     <t>laparoscopy.INTRAABDOMINAL</t>
   </si>
   <si>
-    <t>Endret til med og uten pose</t>
-  </si>
-  <si>
     <t>laparoscopy.MORCELLATOR</t>
   </si>
   <si>
@@ -596,22 +593,38 @@
   </si>
   <si>
     <t>Opf0Status</t>
+  </si>
+  <si>
+    <t>(NB: Noen feilaktig byttet til "LapAdherProfylakse")</t>
+  </si>
+  <si>
+    <t>OpParities</t>
+  </si>
+  <si>
+    <t>OpGraviditeter</t>
+  </si>
+  <si>
+    <t>OpPregnancies</t>
+  </si>
+  <si>
+    <t>OpPariteter</t>
+  </si>
+  <si>
+    <t>OpOptimeCount</t>
+  </si>
+  <si>
+    <t>operation.OPTIME_COUNT</t>
+  </si>
+  <si>
+    <t>OpTid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -664,8 +677,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,11 +983,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B71" sqref="B71:C71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,7 +1003,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C2" t="s">
@@ -998,7 +1011,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
@@ -1006,27 +1019,27 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1034,32 +1047,35 @@
       <c r="A7" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>187</v>
+      <c r="C7" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>192</v>
+      <c r="C8" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1067,10 +1083,10 @@
       <c r="A10" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1078,10 +1094,10 @@
       <c r="A11" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1089,10 +1105,10 @@
       <c r="A12" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1100,10 +1116,10 @@
       <c r="A13" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1111,10 +1127,10 @@
       <c r="A14" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1122,88 +1138,88 @@
       <c r="A15" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>180</v>
+      <c r="C15" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>183</v>
+      <c r="C16" s="2" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>181</v>
+      <c r="C17" s="2" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>182</v>
+      <c r="C18" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>184</v>
+      <c r="C19" s="2" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>185</v>
+      <c r="C20" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1211,10 +1227,10 @@
       <c r="A23" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1222,21 +1238,21 @@
       <c r="A24" t="s">
         <v>97</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>178</v>
+      <c r="C24" s="2" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1244,21 +1260,21 @@
       <c r="A26" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>179</v>
+      <c r="C26" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1266,32 +1282,32 @@
       <c r="A28" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>128</v>
+      <c r="C28" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>103</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>129</v>
+      <c r="C29" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1299,10 +1315,10 @@
       <c r="A31" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1310,261 +1326,262 @@
       <c r="A32" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>131</v>
+      <c r="C32" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>111</v>
-      </c>
-      <c r="B33" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>130</v>
+      <c r="C33" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>123</v>
-      </c>
-      <c r="B34" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" t="s">
-        <v>106</v>
+      <c r="C34" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4" t="s">
-        <v>110</v>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>108</v>
-      </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>47</v>
+      <c r="B37" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>113</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>31</v>
+      <c r="B38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>123</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="4"/>
-      <c r="D40" t="s">
-        <v>188</v>
+        <v>114</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>115</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>40</v>
+      <c r="B41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>116</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>34</v>
+        <v>124</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>125</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>132</v>
+        <v>116</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>117</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>35</v>
+      <c r="B44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>118</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>22</v>
+        <v>120</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>121</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>33</v>
+        <v>118</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>119</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>29</v>
+      <c r="B47" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>120</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>122</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>41</v>
+        <v>123</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>124</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>133</v>
+        <v>95</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>95</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>37</v>
+        <v>126</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>127</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>24</v>
+        <v>125</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>126</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>46</v>
+        <v>134</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>135</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>134</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1572,156 +1589,156 @@
       <c r="A56" t="s">
         <v>136</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>154</v>
+      <c r="B56" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>137</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>13</v>
+        <v>139</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>140</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>155</v>
+        <v>137</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>1</v>
+      <c r="B59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>139</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>177</v>
+        <v>142</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>143</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>160</v>
+        <v>140</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>141</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>162</v>
+        <v>143</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>144</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C63" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>146</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C64" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>145</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C65" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>158</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>147</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>191</v>
+      <c r="B66" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>148</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>161</v>
+        <v>141</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>142</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>12</v>
+        <v>148</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>149</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C69" s="3" t="s">
+      <c r="B69" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>163</v>
       </c>
     </row>
@@ -1729,95 +1746,108 @@
       <c r="A70" t="s">
         <v>150</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>164</v>
+      <c r="B70" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D70" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>151</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D71" t="s">
-        <v>189</v>
+        <v>174</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>175</v>
-      </c>
-      <c r="B72" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>165</v>
+      <c r="C72" s="2" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>175</v>
-      </c>
-      <c r="B73" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C73" s="3" t="s">
-        <v>190</v>
+      <c r="C73" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>175</v>
-      </c>
-      <c r="B74" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C74" s="2" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>175</v>
-      </c>
-      <c r="B75" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>175</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C76" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>175</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>174</v>
+      <c r="B77" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C77" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="1"/>
+      <c r="B78" t="s">
+        <v>196</v>
+      </c>
+      <c r="C78" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>199</v>
+      </c>
+      <c r="B79" t="s">
+        <v>198</v>
+      </c>
+      <c r="C79" t="s">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>